<commit_message>
fix: Update login process and replace hardcoded user ID with parameter
</commit_message>
<xml_diff>
--- a/UsersIPTV.xlsx
+++ b/UsersIPTV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fontes\costumer-notify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE879740-0E02-4506-9E4A-EF632EA28AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1743FD-44D8-4581-84F0-DD78B79AF00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33420" yWindow="1905" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Usuário</t>
   </si>
@@ -69,17 +69,32 @@
   </si>
   <si>
     <t>Telefone</t>
+  </si>
+  <si>
+    <t>F516Z6476b</t>
+  </si>
+  <si>
+    <t>Andressa chies pai e mae</t>
+  </si>
+  <si>
+    <t>5555991539301</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,11 +113,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -114,6 +144,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,7 +652,7 @@
   <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +663,7 @@
     <col min="5" max="5" width="47"/>
     <col min="6" max="6" width="8"/>
     <col min="7" max="7" width="6"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -650,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>983432277</v>
       </c>
@@ -676,8 +718,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H3" s="3"/>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>653559249</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45775.726122685184</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5">
+        <v>10546</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H4" s="3"/>

</xml_diff>